<commit_message>
Error Correction Gantt Diagram
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt del proyecto Integrador.xlsx
+++ b/Diagrama de Gantt del proyecto Integrador.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D7ACA-8409-4D24-85D2-14EA1E1D2BDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2008A93-6B97-4281-8622-A048B61D0BAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="13365" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
@@ -1168,13 +1168,13 @@
                   <c:v>Stablish Teamwork</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Requirement Analisys</c:v>
+                  <c:v>Requirement Analysis</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Project Planning and Control</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Spring Plan Analisys</c:v>
+                  <c:v>Spring Plan Analysis</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Spring 01</c:v>
@@ -1247,7 +1247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDE39445-7F5D-4D9E-AD8B-7AFF20D78EA5}" type="CELLRANGE">
+                    <a:fld id="{5FAFA30B-9810-4607-88E6-CF3140821264}" type="CELLRANGE">
                       <a:rPr lang="es-ES"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1280,7 +1280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F710C040-80EF-4256-8423-7F10D9318BE5}" type="CELLRANGE">
+                    <a:fld id="{11FA7FB0-FAAA-431A-A662-8AB1F856603E}" type="CELLRANGE">
                       <a:rPr lang="es-ES"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1313,7 +1313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4B3CB65-3F6E-4D9F-9362-E27173015E88}" type="CELLRANGE">
+                    <a:fld id="{E920C240-E799-48FA-B930-E11A12073000}" type="CELLRANGE">
                       <a:rPr lang="es-ES"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1417,12 +1417,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.11438382097412635"/>
-                      <c:h val="7.5066274767572133E-2"/>
-                    </c:manualLayout>
-                  </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1438,7 +1432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B77B3C13-F06B-4A69-AC02-4A4A5295AD53}" type="CELLRANGE">
+                    <a:fld id="{00DB2DD3-36E0-4824-9085-4062B9DEF689}" type="CELLRANGE">
                       <a:rPr lang="es-ES"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1523,13 +1517,13 @@
                   <c:v>Stablish Teamwork</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Requirement Analisys</c:v>
+                  <c:v>Requirement Analysis</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Project Planning and Control</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Spring Plan Analisys</c:v>
+                  <c:v>Spring Plan Analysis</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Spring 01</c:v>
@@ -1571,13 +1565,13 @@
                     <c:v>Stablish Teamwork</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Requirement Analisys</c:v>
+                    <c:v>Requirement Analysis</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Project Planning and Control</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Spring Plan Analisys</c:v>
+                    <c:v>Spring Plan Analysis</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>Spring 01</c:v>
@@ -2716,7 +2710,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,8 +2882,8 @@
         <v>43373</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f>"Requirement Analisys"</f>
-        <v>Requirement Analisys</v>
+        <f>"Requirement Analysis"</f>
+        <v>Requirement Analysis</v>
       </c>
       <c r="F9" s="23">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Start Date]])=0,LEN(Hitos[[#This Row],[End Date]])=0),"",INT(C9)-INT($C$6)),"")</f>
@@ -2938,8 +2932,8 @@
         <v>43378</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f>"Spring Plan Analisys"</f>
-        <v>Spring Plan Analisys</v>
+        <f>"Spring Plan Analysis"</f>
+        <v>Spring Plan Analysis</v>
       </c>
       <c r="F11" s="23">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Start Date]])=0,LEN(Hitos[[#This Row],[End Date]])=0),"",INT(C11)-INT($C$6)),"")</f>
@@ -2988,7 +2982,7 @@
         <v>43454</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A8)</f>
+        <f t="shared" ref="E13:E20" si="0">"TBD"&amp;" "&amp;ROW($A8)</f>
         <v>TBD 8</v>
       </c>
       <c r="F13" s="23">
@@ -3013,7 +3007,7 @@
         <v>43423</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A9)</f>
+        <f t="shared" si="0"/>
         <v>TBD 9</v>
       </c>
       <c r="F14" s="23">
@@ -3038,7 +3032,7 @@
         <v>43504</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A10)</f>
+        <f t="shared" si="0"/>
         <v>TBD 10</v>
       </c>
       <c r="F15" s="23">
@@ -3063,7 +3057,7 @@
         <v>43449</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A11)</f>
+        <f t="shared" si="0"/>
         <v>TBD 11</v>
       </c>
       <c r="F16" s="23">
@@ -3088,7 +3082,7 @@
         <v>43501</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A12)</f>
+        <f t="shared" si="0"/>
         <v>TBD 12</v>
       </c>
       <c r="F17" s="23">
@@ -3113,7 +3107,7 @@
         <v>43468</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A13)</f>
+        <f t="shared" si="0"/>
         <v>TBD 13</v>
       </c>
       <c r="F18" s="23">
@@ -3138,7 +3132,7 @@
         <v>43467</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A14)</f>
+        <f t="shared" si="0"/>
         <v>TBD 14</v>
       </c>
       <c r="F19" s="23">
@@ -3163,7 +3157,7 @@
         <v>43521</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f>"TBD"&amp;" "&amp;ROW($A15)</f>
+        <f t="shared" si="0"/>
         <v>TBD 15</v>
       </c>
       <c r="F20" s="23">
@@ -3372,7 +3366,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Follow'!$E7,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Project Follow'!$B7+$B$3,4)),"")</f>
-        <v>Requirement Analisys</v>
+        <v>Requirement Analysis</v>
       </c>
       <c r="C7" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Follow'!$C7,$B$3,0,1,1))=0,End_Date,INDEX(Hitos[],'Project Follow'!$B7+$B$3,2)),"")</f>
@@ -3409,7 +3403,7 @@
       <c r="A9" s="18"/>
       <c r="B9" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Follow'!$E9,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Project Follow'!$B9+$B$3,4)),"")</f>
-        <v>Spring Plan Analisys</v>
+        <v>Spring Plan Analysis</v>
       </c>
       <c r="C9" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Follow'!$C9,$B$3,0,1,1))=0,End_Date,INDEX(Hitos[],'Project Follow'!$B9+$B$3,2)),"")</f>

</xml_diff>